<commit_message>
modify GPlearn and save new results of figure and tables
</commit_message>
<xml_diff>
--- a/Res/gplearn/GPLearn_Results.xlsx
+++ b/Res/gplearn/GPLearn_Results.xlsx
@@ -462,14 +462,14 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.6859</v>
+        <v>0.6411</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1856</v>
+        <v>0.1984</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>abs(add(sqrt(mul(sub(sqrt(sqrt(Ash3)), Ash1), sqrt(mul(Ash0, C_m)))), mul(sub(sub(sqrt(sqrt(sqrt(sub(add(Ash, Ash2), Ash1)))), sqrt(Ash1)), C_m), C_m)))</t>
+          <t>div(div(div(sqrt(sqrt(sqrt(mul(PHS, mul(log(sub(chi, C_m)), r))))), exp(C_0)), exp(C_0)), exp(C_0))</t>
         </is>
       </c>
     </row>

</xml_diff>